<commit_message>
from work machine 28mar22
</commit_message>
<xml_diff>
--- a/10132_Page2.xlsx
+++ b/10132_Page2.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -474,7 +474,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -611,7 +611,7 @@
       </c>
       <c r="J12" s="3" t="inlineStr">
         <is>
-          <t>Modified Marks</t>
+          <t>Team Leader Marks</t>
         </is>
       </c>
     </row>
@@ -1664,7 +1664,7 @@
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>